<commit_message>
updated sample mapping and db file
</commit_message>
<xml_diff>
--- a/bmd2Samps/data/envSampCleanMapping.xlsx
+++ b/bmd2Samps/data/envSampCleanMapping.xlsx
@@ -1,20 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://pnnl-my.sharepoint.com/personal/sara_gosline_pnnl_gov/Documents/Documents/GitHub/srpAnalytics/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://pnnl-my.sharepoint.com/personal/sara_gosline_pnnl_gov/Documents/Documents/GitHub/srpAnalytics/bmd2Samps/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="103" documentId="13_ncr:40009_{9BAE7A55-6E59-42C4-982E-E6B695D3F45E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3EC0C9C9-4542-4019-8C27-BE6C2049C88F}"/>
+  <xr:revisionPtr revIDLastSave="152" documentId="13_ncr:40009_{9BAE7A55-6E59-42C4-982E-E6B695D3F45E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8C8E13FC-37BB-42B3-BB89-12713440B8DE}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2865" yWindow="1800" windowWidth="21600" windowHeight="11325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="envSampCleanMapping" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">envSampCleanMapping!$A$1:$O$132</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -31,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1656" uniqueCount="434">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1656" uniqueCount="433">
   <si>
     <t>10AUG09-01-003</t>
   </si>
@@ -1215,21 +1218,6 @@
     <t>AlternateName</t>
   </si>
   <si>
-    <t>Sample 101</t>
-  </si>
-  <si>
-    <t>Sample 103</t>
-  </si>
-  <si>
-    <t>Sample 1035</t>
-  </si>
-  <si>
-    <t>Sample 1514</t>
-  </si>
-  <si>
-    <t>Sample 1518</t>
-  </si>
-  <si>
     <t>Sample 2791</t>
   </si>
   <si>
@@ -1333,6 +1321,18 @@
   </si>
   <si>
     <t>RM12E-W-S</t>
+  </si>
+  <si>
+    <t>SealCoat_AS A</t>
+  </si>
+  <si>
+    <t>SealCoat_1.6 h C</t>
+  </si>
+  <si>
+    <t>SealCoat_CT-1 A</t>
+  </si>
+  <si>
+    <t>SealCoat_CT-2 A</t>
   </si>
 </sst>
 </file>
@@ -2177,8 +2177,8 @@
   <dimension ref="A1:O132"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A106" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N113" sqref="N113"/>
+      <pane ySplit="1" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C54" sqref="C54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2238,13 +2238,13 @@
         <v>393</v>
       </c>
       <c r="M1" t="s">
-        <v>421</v>
+        <v>416</v>
       </c>
       <c r="N1" t="s">
-        <v>408</v>
+        <v>403</v>
       </c>
       <c r="O1" t="s">
-        <v>409</v>
+        <v>404</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
@@ -2285,7 +2285,7 @@
         <v>33</v>
       </c>
       <c r="M2" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
       <c r="N2" t="s">
         <v>31</v>
@@ -2332,7 +2332,7 @@
         <v>33</v>
       </c>
       <c r="M3" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
       <c r="N3" t="s">
         <v>111</v>
@@ -2379,7 +2379,7 @@
         <v>33</v>
       </c>
       <c r="M4" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
       <c r="N4" t="s">
         <v>136</v>
@@ -2426,7 +2426,7 @@
         <v>33</v>
       </c>
       <c r="M5" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
       <c r="N5" t="s">
         <v>177</v>
@@ -2473,7 +2473,7 @@
         <v>33</v>
       </c>
       <c r="M6" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
       <c r="N6" t="s">
         <v>197</v>
@@ -2520,7 +2520,7 @@
         <v>33</v>
       </c>
       <c r="M7" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
       <c r="N7" t="s">
         <v>223</v>
@@ -2567,7 +2567,7 @@
         <v>38</v>
       </c>
       <c r="M8" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
       <c r="N8" t="s">
         <v>36</v>
@@ -2614,7 +2614,7 @@
         <v>38</v>
       </c>
       <c r="M9" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
       <c r="N9" t="s">
         <v>114</v>
@@ -2661,7 +2661,7 @@
         <v>38</v>
       </c>
       <c r="M10" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
       <c r="N10" t="s">
         <v>140</v>
@@ -2708,7 +2708,7 @@
         <v>38</v>
       </c>
       <c r="M11" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
       <c r="N11" t="s">
         <v>199</v>
@@ -2755,7 +2755,7 @@
         <v>38</v>
       </c>
       <c r="M12" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
       <c r="N12" t="s">
         <v>225</v>
@@ -2799,7 +2799,7 @@
         <v>4</v>
       </c>
       <c r="M13" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
       <c r="N13" t="s">
         <v>27</v>
@@ -2843,7 +2843,7 @@
         <v>4</v>
       </c>
       <c r="M14" t="s">
-        <v>410</v>
+        <v>405</v>
       </c>
       <c r="N14" t="s">
         <v>88</v>
@@ -2887,7 +2887,7 @@
         <v>4</v>
       </c>
       <c r="M15" t="s">
-        <v>410</v>
+        <v>405</v>
       </c>
       <c r="N15" t="s">
         <v>100</v>
@@ -2931,7 +2931,7 @@
         <v>4</v>
       </c>
       <c r="M16" t="s">
-        <v>410</v>
+        <v>405</v>
       </c>
       <c r="N16" t="s">
         <v>107</v>
@@ -2975,7 +2975,7 @@
         <v>4</v>
       </c>
       <c r="M17" t="s">
-        <v>410</v>
+        <v>405</v>
       </c>
       <c r="N17" t="s">
         <v>173</v>
@@ -3019,7 +3019,7 @@
         <v>4</v>
       </c>
       <c r="M18" t="s">
-        <v>410</v>
+        <v>405</v>
       </c>
       <c r="N18" t="s">
         <v>259</v>
@@ -3063,7 +3063,7 @@
         <v>4</v>
       </c>
       <c r="M19" t="s">
-        <v>410</v>
+        <v>405</v>
       </c>
       <c r="N19" t="s">
         <v>270</v>
@@ -3107,7 +3107,7 @@
         <v>4</v>
       </c>
       <c r="M20" t="s">
-        <v>410</v>
+        <v>405</v>
       </c>
       <c r="N20" t="s">
         <v>277</v>
@@ -3124,10 +3124,10 @@
         <v>326</v>
       </c>
       <c r="C21" t="s">
-        <v>326</v>
+        <v>338</v>
       </c>
       <c r="D21" t="s">
-        <v>326</v>
+        <v>339</v>
       </c>
       <c r="E21" s="1">
         <v>1520</v>
@@ -3154,7 +3154,7 @@
         <v>330</v>
       </c>
       <c r="M21" t="s">
-        <v>413</v>
+        <v>408</v>
       </c>
       <c r="N21" t="s">
         <v>328</v>
@@ -3171,10 +3171,10 @@
         <v>326</v>
       </c>
       <c r="C22" t="s">
-        <v>326</v>
+        <v>338</v>
       </c>
       <c r="D22" t="s">
-        <v>326</v>
+        <v>339</v>
       </c>
       <c r="E22" s="1">
         <v>1521</v>
@@ -3201,7 +3201,7 @@
         <v>330</v>
       </c>
       <c r="M22" t="s">
-        <v>413</v>
+        <v>408</v>
       </c>
       <c r="N22" t="s">
         <v>332</v>
@@ -3218,10 +3218,10 @@
         <v>326</v>
       </c>
       <c r="C23" t="s">
-        <v>326</v>
+        <v>338</v>
       </c>
       <c r="D23" t="s">
-        <v>326</v>
+        <v>339</v>
       </c>
       <c r="E23" s="1">
         <v>1519</v>
@@ -3248,7 +3248,7 @@
         <v>330</v>
       </c>
       <c r="M23" t="s">
-        <v>413</v>
+        <v>408</v>
       </c>
       <c r="N23" t="s">
         <v>372</v>
@@ -3292,7 +3292,7 @@
         <v>4</v>
       </c>
       <c r="M24" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
       <c r="N24" t="s">
         <v>5</v>
@@ -3336,7 +3336,7 @@
         <v>4</v>
       </c>
       <c r="M25" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
       <c r="N25" t="s">
         <v>19</v>
@@ -3380,7 +3380,7 @@
         <v>4</v>
       </c>
       <c r="M26" t="s">
-        <v>410</v>
+        <v>405</v>
       </c>
       <c r="N26" t="s">
         <v>80</v>
@@ -3424,7 +3424,7 @@
         <v>4</v>
       </c>
       <c r="M27" t="s">
-        <v>410</v>
+        <v>405</v>
       </c>
       <c r="N27" t="s">
         <v>94</v>
@@ -3468,7 +3468,7 @@
         <v>4</v>
       </c>
       <c r="M28" t="s">
-        <v>410</v>
+        <v>405</v>
       </c>
       <c r="N28" t="s">
         <v>165</v>
@@ -3512,7 +3512,7 @@
         <v>4</v>
       </c>
       <c r="M29" t="s">
-        <v>410</v>
+        <v>405</v>
       </c>
       <c r="N29" t="s">
         <v>263</v>
@@ -3556,7 +3556,7 @@
         <v>4</v>
       </c>
       <c r="M30" t="s">
-        <v>410</v>
+        <v>405</v>
       </c>
       <c r="N30" t="s">
         <v>273</v>
@@ -3600,7 +3600,7 @@
         <v>4</v>
       </c>
       <c r="M31" t="s">
-        <v>410</v>
+        <v>405</v>
       </c>
       <c r="N31" t="s">
         <v>283</v>
@@ -3644,7 +3644,7 @@
         <v>4</v>
       </c>
       <c r="M32" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
       <c r="N32" t="s">
         <v>10</v>
@@ -3688,7 +3688,7 @@
         <v>4</v>
       </c>
       <c r="M33" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
       <c r="N33" t="s">
         <v>23</v>
@@ -3732,7 +3732,7 @@
         <v>4</v>
       </c>
       <c r="M34" t="s">
-        <v>410</v>
+        <v>405</v>
       </c>
       <c r="N34" t="s">
         <v>84</v>
@@ -3776,7 +3776,7 @@
         <v>4</v>
       </c>
       <c r="M35" t="s">
-        <v>410</v>
+        <v>405</v>
       </c>
       <c r="N35" t="s">
         <v>97</v>
@@ -3820,7 +3820,7 @@
         <v>4</v>
       </c>
       <c r="M36" t="s">
-        <v>410</v>
+        <v>405</v>
       </c>
       <c r="N36" t="s">
         <v>169</v>
@@ -3864,7 +3864,7 @@
         <v>4</v>
       </c>
       <c r="M37" t="s">
-        <v>410</v>
+        <v>405</v>
       </c>
       <c r="N37" t="s">
         <v>279</v>
@@ -3881,10 +3881,10 @@
         <v>326</v>
       </c>
       <c r="C38" t="s">
-        <v>326</v>
+        <v>338</v>
       </c>
       <c r="D38" t="s">
-        <v>326</v>
+        <v>339</v>
       </c>
       <c r="E38" s="1">
         <v>1037</v>
@@ -3908,7 +3908,7 @@
         <v>327</v>
       </c>
       <c r="M38" t="s">
-        <v>413</v>
+        <v>408</v>
       </c>
       <c r="N38" t="s">
         <v>347</v>
@@ -3925,10 +3925,10 @@
         <v>326</v>
       </c>
       <c r="C39" t="s">
-        <v>326</v>
+        <v>338</v>
       </c>
       <c r="D39" t="s">
-        <v>326</v>
+        <v>339</v>
       </c>
       <c r="E39" s="1">
         <v>1038</v>
@@ -3952,7 +3952,7 @@
         <v>327</v>
       </c>
       <c r="M39" t="s">
-        <v>413</v>
+        <v>408</v>
       </c>
       <c r="N39" t="s">
         <v>362</v>
@@ -3969,10 +3969,10 @@
         <v>326</v>
       </c>
       <c r="C40" t="s">
-        <v>326</v>
+        <v>338</v>
       </c>
       <c r="D40" t="s">
-        <v>326</v>
+        <v>339</v>
       </c>
       <c r="E40" s="1">
         <v>1036</v>
@@ -3996,7 +3996,7 @@
         <v>327</v>
       </c>
       <c r="M40" t="s">
-        <v>413</v>
+        <v>408</v>
       </c>
       <c r="N40" t="s">
         <v>377</v>
@@ -4043,7 +4043,7 @@
         <v>293</v>
       </c>
       <c r="M41" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
       <c r="N41" t="s">
         <v>291</v>
@@ -4090,10 +4090,10 @@
         <v>293</v>
       </c>
       <c r="M42" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
       <c r="N42" t="s">
-        <v>422</v>
+        <v>417</v>
       </c>
       <c r="O42" t="s">
         <v>292</v>
@@ -4137,10 +4137,10 @@
         <v>58</v>
       </c>
       <c r="M43" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
       <c r="N43" t="s">
-        <v>423</v>
+        <v>418</v>
       </c>
       <c r="O43" t="s">
         <v>57</v>
@@ -4184,7 +4184,7 @@
         <v>58</v>
       </c>
       <c r="M44" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
       <c r="N44" t="s">
         <v>123</v>
@@ -4231,7 +4231,7 @@
         <v>58</v>
       </c>
       <c r="M45" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
       <c r="N45" t="s">
         <v>149</v>
@@ -4278,7 +4278,7 @@
         <v>58</v>
       </c>
       <c r="M46" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
       <c r="N46" t="s">
         <v>189</v>
@@ -4325,7 +4325,7 @@
         <v>58</v>
       </c>
       <c r="M47" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
       <c r="N47" t="s">
         <v>209</v>
@@ -4372,7 +4372,7 @@
         <v>58</v>
       </c>
       <c r="M48" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
       <c r="N48" t="s">
         <v>236</v>
@@ -4389,19 +4389,19 @@
         <v>327</v>
       </c>
       <c r="C49" t="s">
-        <v>327</v>
+        <v>338</v>
       </c>
       <c r="D49" t="s">
-        <v>327</v>
+        <v>339</v>
       </c>
       <c r="E49" s="1">
         <v>101</v>
       </c>
       <c r="F49" t="s">
-        <v>327</v>
+        <v>356</v>
       </c>
       <c r="G49" t="s">
-        <v>394</v>
+        <v>374</v>
       </c>
       <c r="H49" t="s">
         <v>327</v>
@@ -4410,22 +4410,22 @@
         <v>327</v>
       </c>
       <c r="J49" t="s">
-        <v>326</v>
+        <v>356</v>
       </c>
       <c r="K49" t="s">
         <v>327</v>
       </c>
       <c r="L49" t="s">
-        <v>327</v>
+        <v>375</v>
       </c>
       <c r="M49" t="s">
-        <v>414</v>
+        <v>356</v>
       </c>
       <c r="N49" t="s">
-        <v>394</v>
+        <v>374</v>
       </c>
       <c r="O49" t="s">
-        <v>414</v>
+        <v>356</v>
       </c>
     </row>
     <row r="50" spans="1:15" x14ac:dyDescent="0.25">
@@ -4436,19 +4436,19 @@
         <v>327</v>
       </c>
       <c r="C50" t="s">
-        <v>327</v>
+        <v>338</v>
       </c>
       <c r="D50" t="s">
-        <v>327</v>
+        <v>339</v>
       </c>
       <c r="E50" s="1">
         <v>103</v>
       </c>
       <c r="F50" t="s">
-        <v>327</v>
+        <v>356</v>
       </c>
       <c r="G50" t="s">
-        <v>395</v>
+        <v>430</v>
       </c>
       <c r="H50" t="s">
         <v>327</v>
@@ -4457,22 +4457,22 @@
         <v>327</v>
       </c>
       <c r="J50" t="s">
-        <v>326</v>
+        <v>356</v>
       </c>
       <c r="K50" t="s">
         <v>327</v>
       </c>
       <c r="L50" t="s">
-        <v>327</v>
+        <v>375</v>
       </c>
       <c r="M50" t="s">
-        <v>414</v>
+        <v>356</v>
       </c>
       <c r="N50" t="s">
-        <v>395</v>
+        <v>430</v>
       </c>
       <c r="O50" t="s">
-        <v>414</v>
+        <v>356</v>
       </c>
     </row>
     <row r="51" spans="1:15" x14ac:dyDescent="0.25">
@@ -4483,19 +4483,19 @@
         <v>327</v>
       </c>
       <c r="C51" t="s">
-        <v>327</v>
+        <v>338</v>
       </c>
       <c r="D51" t="s">
-        <v>327</v>
+        <v>339</v>
       </c>
       <c r="E51" s="1">
         <v>1035</v>
       </c>
       <c r="F51" t="s">
-        <v>327</v>
+        <v>348</v>
       </c>
       <c r="G51" t="s">
-        <v>396</v>
+        <v>429</v>
       </c>
       <c r="H51" t="s">
         <v>327</v>
@@ -4504,7 +4504,7 @@
         <v>327</v>
       </c>
       <c r="J51" t="s">
-        <v>326</v>
+        <v>348</v>
       </c>
       <c r="K51" t="s">
         <v>327</v>
@@ -4513,13 +4513,13 @@
         <v>327</v>
       </c>
       <c r="M51" t="s">
-        <v>414</v>
+        <v>348</v>
       </c>
       <c r="N51" t="s">
-        <v>396</v>
+        <v>429</v>
       </c>
       <c r="O51" t="s">
-        <v>414</v>
+        <v>348</v>
       </c>
     </row>
     <row r="52" spans="1:15" x14ac:dyDescent="0.25">
@@ -4530,19 +4530,19 @@
         <v>327</v>
       </c>
       <c r="C52" t="s">
-        <v>327</v>
+        <v>338</v>
       </c>
       <c r="D52" t="s">
-        <v>327</v>
+        <v>339</v>
       </c>
       <c r="E52" s="1">
         <v>1514</v>
       </c>
       <c r="F52" t="s">
-        <v>327</v>
+        <v>356</v>
       </c>
       <c r="G52" t="s">
-        <v>397</v>
+        <v>431</v>
       </c>
       <c r="H52" t="s">
         <v>327</v>
@@ -4551,22 +4551,22 @@
         <v>327</v>
       </c>
       <c r="J52" t="s">
-        <v>326</v>
+        <v>356</v>
       </c>
       <c r="K52" t="s">
         <v>327</v>
       </c>
       <c r="L52" t="s">
-        <v>327</v>
+        <v>357</v>
       </c>
       <c r="M52" t="s">
-        <v>414</v>
+        <v>356</v>
       </c>
       <c r="N52" t="s">
-        <v>397</v>
+        <v>431</v>
       </c>
       <c r="O52" t="s">
-        <v>414</v>
+        <v>356</v>
       </c>
     </row>
     <row r="53" spans="1:15" x14ac:dyDescent="0.25">
@@ -4577,19 +4577,19 @@
         <v>327</v>
       </c>
       <c r="C53" t="s">
-        <v>327</v>
+        <v>338</v>
       </c>
       <c r="D53" t="s">
-        <v>327</v>
+        <v>339</v>
       </c>
       <c r="E53" s="1">
         <v>1518</v>
       </c>
       <c r="F53" t="s">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="G53" t="s">
-        <v>398</v>
+        <v>432</v>
       </c>
       <c r="H53" t="s">
         <v>327</v>
@@ -4598,22 +4598,22 @@
         <v>327</v>
       </c>
       <c r="J53" t="s">
-        <v>326</v>
+        <v>329</v>
       </c>
       <c r="K53" t="s">
         <v>327</v>
       </c>
       <c r="L53" t="s">
-        <v>327</v>
+        <v>330</v>
       </c>
       <c r="M53" t="s">
-        <v>414</v>
+        <v>329</v>
       </c>
       <c r="N53" t="s">
-        <v>398</v>
+        <v>432</v>
       </c>
       <c r="O53" t="s">
-        <v>414</v>
+        <v>329</v>
       </c>
     </row>
     <row r="54" spans="1:15" x14ac:dyDescent="0.25">
@@ -4624,10 +4624,10 @@
         <v>327</v>
       </c>
       <c r="C54" t="s">
-        <v>327</v>
+        <v>338</v>
       </c>
       <c r="D54" t="s">
-        <v>327</v>
+        <v>339</v>
       </c>
       <c r="E54" s="1">
         <v>2791</v>
@@ -4636,7 +4636,7 @@
         <v>327</v>
       </c>
       <c r="G54" t="s">
-        <v>399</v>
+        <v>394</v>
       </c>
       <c r="H54" t="s">
         <v>327</v>
@@ -4654,13 +4654,13 @@
         <v>327</v>
       </c>
       <c r="M54" t="s">
-        <v>414</v>
+        <v>409</v>
       </c>
       <c r="N54" t="s">
-        <v>399</v>
+        <v>394</v>
       </c>
       <c r="O54" t="s">
-        <v>414</v>
+        <v>409</v>
       </c>
     </row>
     <row r="55" spans="1:15" x14ac:dyDescent="0.25">
@@ -4671,10 +4671,10 @@
         <v>327</v>
       </c>
       <c r="C55" t="s">
-        <v>327</v>
+        <v>338</v>
       </c>
       <c r="D55" t="s">
-        <v>327</v>
+        <v>339</v>
       </c>
       <c r="E55" s="1">
         <v>3053</v>
@@ -4683,7 +4683,7 @@
         <v>327</v>
       </c>
       <c r="G55" t="s">
-        <v>400</v>
+        <v>395</v>
       </c>
       <c r="H55" t="s">
         <v>327</v>
@@ -4701,13 +4701,13 @@
         <v>327</v>
       </c>
       <c r="M55" t="s">
-        <v>414</v>
+        <v>409</v>
       </c>
       <c r="N55" t="s">
-        <v>400</v>
+        <v>395</v>
       </c>
       <c r="O55" t="s">
-        <v>414</v>
+        <v>409</v>
       </c>
     </row>
     <row r="56" spans="1:15" x14ac:dyDescent="0.25">
@@ -4718,10 +4718,10 @@
         <v>327</v>
       </c>
       <c r="C56" t="s">
-        <v>327</v>
+        <v>338</v>
       </c>
       <c r="D56" t="s">
-        <v>327</v>
+        <v>339</v>
       </c>
       <c r="E56" s="1">
         <v>3328</v>
@@ -4730,7 +4730,7 @@
         <v>327</v>
       </c>
       <c r="G56" t="s">
-        <v>401</v>
+        <v>396</v>
       </c>
       <c r="H56" t="s">
         <v>327</v>
@@ -4748,13 +4748,13 @@
         <v>327</v>
       </c>
       <c r="M56" t="s">
-        <v>414</v>
+        <v>409</v>
       </c>
       <c r="N56" t="s">
-        <v>401</v>
+        <v>396</v>
       </c>
       <c r="O56" t="s">
-        <v>414</v>
+        <v>409</v>
       </c>
     </row>
     <row r="57" spans="1:15" x14ac:dyDescent="0.25">
@@ -4765,10 +4765,10 @@
         <v>327</v>
       </c>
       <c r="C57" t="s">
-        <v>327</v>
+        <v>338</v>
       </c>
       <c r="D57" t="s">
-        <v>327</v>
+        <v>339</v>
       </c>
       <c r="E57" s="1">
         <v>3329</v>
@@ -4777,7 +4777,7 @@
         <v>327</v>
       </c>
       <c r="G57" t="s">
-        <v>402</v>
+        <v>397</v>
       </c>
       <c r="H57" t="s">
         <v>327</v>
@@ -4795,13 +4795,13 @@
         <v>327</v>
       </c>
       <c r="M57" t="s">
-        <v>414</v>
+        <v>409</v>
       </c>
       <c r="N57" t="s">
-        <v>402</v>
+        <v>397</v>
       </c>
       <c r="O57" t="s">
-        <v>414</v>
+        <v>409</v>
       </c>
     </row>
     <row r="58" spans="1:15" x14ac:dyDescent="0.25">
@@ -4812,10 +4812,10 @@
         <v>327</v>
       </c>
       <c r="C58" t="s">
-        <v>327</v>
+        <v>338</v>
       </c>
       <c r="D58" t="s">
-        <v>327</v>
+        <v>339</v>
       </c>
       <c r="E58" s="1">
         <v>3332</v>
@@ -4824,7 +4824,7 @@
         <v>327</v>
       </c>
       <c r="G58" t="s">
-        <v>403</v>
+        <v>398</v>
       </c>
       <c r="H58" t="s">
         <v>327</v>
@@ -4842,13 +4842,13 @@
         <v>327</v>
       </c>
       <c r="M58" t="s">
-        <v>414</v>
+        <v>409</v>
       </c>
       <c r="N58" t="s">
-        <v>403</v>
+        <v>398</v>
       </c>
       <c r="O58" t="s">
-        <v>414</v>
+        <v>409</v>
       </c>
     </row>
     <row r="59" spans="1:15" x14ac:dyDescent="0.25">
@@ -4859,10 +4859,10 @@
         <v>327</v>
       </c>
       <c r="C59" t="s">
-        <v>327</v>
+        <v>338</v>
       </c>
       <c r="D59" t="s">
-        <v>327</v>
+        <v>339</v>
       </c>
       <c r="E59" s="1">
         <v>3334</v>
@@ -4871,7 +4871,7 @@
         <v>327</v>
       </c>
       <c r="G59" t="s">
-        <v>404</v>
+        <v>399</v>
       </c>
       <c r="H59" t="s">
         <v>327</v>
@@ -4889,13 +4889,13 @@
         <v>327</v>
       </c>
       <c r="M59" t="s">
-        <v>414</v>
+        <v>409</v>
       </c>
       <c r="N59" t="s">
-        <v>404</v>
+        <v>399</v>
       </c>
       <c r="O59" t="s">
-        <v>414</v>
+        <v>409</v>
       </c>
     </row>
     <row r="60" spans="1:15" x14ac:dyDescent="0.25">
@@ -4906,10 +4906,10 @@
         <v>327</v>
       </c>
       <c r="C60" t="s">
-        <v>327</v>
+        <v>338</v>
       </c>
       <c r="D60" t="s">
-        <v>327</v>
+        <v>339</v>
       </c>
       <c r="E60" s="1">
         <v>889</v>
@@ -4918,7 +4918,7 @@
         <v>327</v>
       </c>
       <c r="G60" t="s">
-        <v>405</v>
+        <v>400</v>
       </c>
       <c r="H60" t="s">
         <v>327</v>
@@ -4936,13 +4936,13 @@
         <v>327</v>
       </c>
       <c r="M60" t="s">
-        <v>414</v>
+        <v>409</v>
       </c>
       <c r="N60" t="s">
-        <v>405</v>
+        <v>400</v>
       </c>
       <c r="O60" t="s">
-        <v>414</v>
+        <v>409</v>
       </c>
     </row>
     <row r="61" spans="1:15" x14ac:dyDescent="0.25">
@@ -4953,10 +4953,10 @@
         <v>327</v>
       </c>
       <c r="C61" t="s">
-        <v>327</v>
+        <v>338</v>
       </c>
       <c r="D61" t="s">
-        <v>327</v>
+        <v>339</v>
       </c>
       <c r="E61" s="1">
         <v>890</v>
@@ -4965,7 +4965,7 @@
         <v>327</v>
       </c>
       <c r="G61" t="s">
-        <v>406</v>
+        <v>401</v>
       </c>
       <c r="H61" t="s">
         <v>327</v>
@@ -4983,13 +4983,13 @@
         <v>327</v>
       </c>
       <c r="M61" t="s">
-        <v>414</v>
+        <v>409</v>
       </c>
       <c r="N61" t="s">
-        <v>406</v>
+        <v>401</v>
       </c>
       <c r="O61" t="s">
-        <v>414</v>
+        <v>409</v>
       </c>
     </row>
     <row r="62" spans="1:15" x14ac:dyDescent="0.25">
@@ -5000,10 +5000,10 @@
         <v>327</v>
       </c>
       <c r="C62" t="s">
-        <v>327</v>
+        <v>338</v>
       </c>
       <c r="D62" t="s">
-        <v>327</v>
+        <v>339</v>
       </c>
       <c r="E62" s="1">
         <v>891</v>
@@ -5012,7 +5012,7 @@
         <v>327</v>
       </c>
       <c r="G62" t="s">
-        <v>407</v>
+        <v>402</v>
       </c>
       <c r="H62" t="s">
         <v>327</v>
@@ -5030,13 +5030,13 @@
         <v>327</v>
       </c>
       <c r="M62" t="s">
-        <v>414</v>
+        <v>409</v>
       </c>
       <c r="N62" t="s">
-        <v>407</v>
+        <v>402</v>
       </c>
       <c r="O62" t="s">
-        <v>414</v>
+        <v>409</v>
       </c>
     </row>
     <row r="63" spans="1:15" x14ac:dyDescent="0.25">
@@ -5074,7 +5074,7 @@
         <v>4</v>
       </c>
       <c r="M63" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
       <c r="N63" t="s">
         <v>14</v>
@@ -5118,7 +5118,7 @@
         <v>4</v>
       </c>
       <c r="M64" t="s">
-        <v>410</v>
+        <v>405</v>
       </c>
       <c r="N64" t="s">
         <v>76</v>
@@ -5162,7 +5162,7 @@
         <v>4</v>
       </c>
       <c r="M65" t="s">
-        <v>410</v>
+        <v>405</v>
       </c>
       <c r="N65" t="s">
         <v>91</v>
@@ -5206,7 +5206,7 @@
         <v>4</v>
       </c>
       <c r="M66" t="s">
-        <v>410</v>
+        <v>405</v>
       </c>
       <c r="N66" t="s">
         <v>103</v>
@@ -5250,7 +5250,7 @@
         <v>4</v>
       </c>
       <c r="M67" t="s">
-        <v>410</v>
+        <v>405</v>
       </c>
       <c r="N67" t="s">
         <v>161</v>
@@ -5294,7 +5294,7 @@
         <v>4</v>
       </c>
       <c r="M68" t="s">
-        <v>410</v>
+        <v>405</v>
       </c>
       <c r="N68" t="s">
         <v>266</v>
@@ -5338,7 +5338,7 @@
         <v>4</v>
       </c>
       <c r="M69" t="s">
-        <v>410</v>
+        <v>405</v>
       </c>
       <c r="N69" t="s">
         <v>287</v>
@@ -5385,13 +5385,13 @@
         <v>63</v>
       </c>
       <c r="M70" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
       <c r="N70" t="s">
-        <v>424</v>
+        <v>419</v>
       </c>
       <c r="O70" t="s">
-        <v>415</v>
+        <v>410</v>
       </c>
     </row>
     <row r="71" spans="1:15" x14ac:dyDescent="0.25">
@@ -5432,13 +5432,13 @@
         <v>63</v>
       </c>
       <c r="M71" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
       <c r="N71" t="s">
         <v>126</v>
       </c>
       <c r="O71" t="s">
-        <v>415</v>
+        <v>410</v>
       </c>
     </row>
     <row r="72" spans="1:15" x14ac:dyDescent="0.25">
@@ -5479,13 +5479,13 @@
         <v>63</v>
       </c>
       <c r="M72" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
       <c r="N72" t="s">
         <v>152</v>
       </c>
       <c r="O72" t="s">
-        <v>415</v>
+        <v>410</v>
       </c>
     </row>
     <row r="73" spans="1:15" x14ac:dyDescent="0.25">
@@ -5526,13 +5526,13 @@
         <v>63</v>
       </c>
       <c r="M73" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
       <c r="N73" t="s">
         <v>212</v>
       </c>
       <c r="O73" t="s">
-        <v>415</v>
+        <v>410</v>
       </c>
     </row>
     <row r="74" spans="1:15" x14ac:dyDescent="0.25">
@@ -5573,13 +5573,13 @@
         <v>63</v>
       </c>
       <c r="M74" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
       <c r="N74" t="s">
         <v>215</v>
       </c>
       <c r="O74" t="s">
-        <v>415</v>
+        <v>410</v>
       </c>
     </row>
     <row r="75" spans="1:15" x14ac:dyDescent="0.25">
@@ -5620,13 +5620,13 @@
         <v>63</v>
       </c>
       <c r="M75" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
       <c r="N75" t="s">
         <v>218</v>
       </c>
       <c r="O75" t="s">
-        <v>415</v>
+        <v>410</v>
       </c>
     </row>
     <row r="76" spans="1:15" x14ac:dyDescent="0.25">
@@ -5667,13 +5667,13 @@
         <v>63</v>
       </c>
       <c r="M76" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
       <c r="N76" t="s">
         <v>240</v>
       </c>
       <c r="O76" t="s">
-        <v>415</v>
+        <v>410</v>
       </c>
     </row>
     <row r="77" spans="1:15" x14ac:dyDescent="0.25">
@@ -5714,13 +5714,13 @@
         <v>63</v>
       </c>
       <c r="M77" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
       <c r="N77" t="s">
         <v>243</v>
       </c>
       <c r="O77" t="s">
-        <v>415</v>
+        <v>410</v>
       </c>
     </row>
     <row r="78" spans="1:15" x14ac:dyDescent="0.25">
@@ -5761,13 +5761,13 @@
         <v>63</v>
       </c>
       <c r="M78" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
       <c r="N78" t="s">
         <v>246</v>
       </c>
       <c r="O78" t="s">
-        <v>415</v>
+        <v>410</v>
       </c>
     </row>
     <row r="79" spans="1:15" x14ac:dyDescent="0.25">
@@ -5808,13 +5808,13 @@
         <v>63</v>
       </c>
       <c r="M79" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
       <c r="N79" t="s">
         <v>249</v>
       </c>
       <c r="O79" t="s">
-        <v>415</v>
+        <v>410</v>
       </c>
     </row>
     <row r="80" spans="1:15" x14ac:dyDescent="0.25">
@@ -5855,13 +5855,13 @@
         <v>63</v>
       </c>
       <c r="M80" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
       <c r="N80" t="s">
         <v>252</v>
       </c>
       <c r="O80" t="s">
-        <v>415</v>
+        <v>410</v>
       </c>
     </row>
     <row r="81" spans="1:15" x14ac:dyDescent="0.25">
@@ -5902,13 +5902,13 @@
         <v>302</v>
       </c>
       <c r="M81" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
       <c r="N81" t="s">
         <v>299</v>
       </c>
       <c r="O81" t="s">
-        <v>420</v>
+        <v>415</v>
       </c>
     </row>
     <row r="82" spans="1:15" x14ac:dyDescent="0.25">
@@ -5949,13 +5949,13 @@
         <v>302</v>
       </c>
       <c r="M82" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
       <c r="N82" t="s">
-        <v>425</v>
+        <v>420</v>
       </c>
       <c r="O82" t="s">
-        <v>420</v>
+        <v>415</v>
       </c>
     </row>
     <row r="83" spans="1:15" x14ac:dyDescent="0.25">
@@ -5996,7 +5996,7 @@
         <v>308</v>
       </c>
       <c r="M83" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
       <c r="N83" t="s">
         <v>305</v>
@@ -6043,10 +6043,10 @@
         <v>308</v>
       </c>
       <c r="M84" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
       <c r="N84" t="s">
-        <v>426</v>
+        <v>421</v>
       </c>
       <c r="O84" t="s">
         <v>307</v>
@@ -6090,7 +6090,7 @@
         <v>308</v>
       </c>
       <c r="M85" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
       <c r="N85" t="s">
         <v>324</v>
@@ -6137,13 +6137,13 @@
         <v>68</v>
       </c>
       <c r="M86" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
       <c r="N86" t="s">
-        <v>427</v>
+        <v>422</v>
       </c>
       <c r="O86" t="s">
-        <v>419</v>
+        <v>414</v>
       </c>
     </row>
     <row r="87" spans="1:15" x14ac:dyDescent="0.25">
@@ -6184,13 +6184,13 @@
         <v>68</v>
       </c>
       <c r="M87" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
       <c r="N87" t="s">
         <v>129</v>
       </c>
       <c r="O87" t="s">
-        <v>419</v>
+        <v>414</v>
       </c>
     </row>
     <row r="88" spans="1:15" x14ac:dyDescent="0.25">
@@ -6231,13 +6231,13 @@
         <v>68</v>
       </c>
       <c r="M88" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
       <c r="N88" t="s">
         <v>155</v>
       </c>
       <c r="O88" t="s">
-        <v>419</v>
+        <v>414</v>
       </c>
     </row>
     <row r="89" spans="1:15" x14ac:dyDescent="0.25">
@@ -6278,13 +6278,13 @@
         <v>68</v>
       </c>
       <c r="M89" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
       <c r="N89" t="s">
         <v>192</v>
       </c>
       <c r="O89" t="s">
-        <v>419</v>
+        <v>414</v>
       </c>
     </row>
     <row r="90" spans="1:15" x14ac:dyDescent="0.25">
@@ -6325,13 +6325,13 @@
         <v>68</v>
       </c>
       <c r="M90" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
       <c r="N90" t="s">
         <v>207</v>
       </c>
       <c r="O90" t="s">
-        <v>419</v>
+        <v>414</v>
       </c>
     </row>
     <row r="91" spans="1:15" x14ac:dyDescent="0.25">
@@ -6372,13 +6372,13 @@
         <v>68</v>
       </c>
       <c r="M91" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
       <c r="N91" t="s">
         <v>234</v>
       </c>
       <c r="O91" t="s">
-        <v>419</v>
+        <v>414</v>
       </c>
     </row>
     <row r="92" spans="1:15" x14ac:dyDescent="0.25">
@@ -6419,13 +6419,13 @@
         <v>43</v>
       </c>
       <c r="M92" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
       <c r="N92" t="s">
-        <v>428</v>
+        <v>423</v>
       </c>
       <c r="O92" t="s">
-        <v>412</v>
+        <v>407</v>
       </c>
     </row>
     <row r="93" spans="1:15" x14ac:dyDescent="0.25">
@@ -6466,13 +6466,13 @@
         <v>43</v>
       </c>
       <c r="M93" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
       <c r="N93" t="s">
         <v>117</v>
       </c>
       <c r="O93" t="s">
-        <v>412</v>
+        <v>407</v>
       </c>
     </row>
     <row r="94" spans="1:15" x14ac:dyDescent="0.25">
@@ -6513,13 +6513,13 @@
         <v>43</v>
       </c>
       <c r="M94" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
       <c r="N94" t="s">
         <v>143</v>
       </c>
       <c r="O94" t="s">
-        <v>412</v>
+        <v>407</v>
       </c>
     </row>
     <row r="95" spans="1:15" x14ac:dyDescent="0.25">
@@ -6560,13 +6560,13 @@
         <v>43</v>
       </c>
       <c r="M95" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
       <c r="N95" t="s">
         <v>183</v>
       </c>
       <c r="O95" t="s">
-        <v>412</v>
+        <v>407</v>
       </c>
     </row>
     <row r="96" spans="1:15" x14ac:dyDescent="0.25">
@@ -6607,13 +6607,13 @@
         <v>43</v>
       </c>
       <c r="M96" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
       <c r="N96" t="s">
         <v>201</v>
       </c>
       <c r="O96" t="s">
-        <v>412</v>
+        <v>407</v>
       </c>
     </row>
     <row r="97" spans="1:15" x14ac:dyDescent="0.25">
@@ -6654,13 +6654,13 @@
         <v>43</v>
       </c>
       <c r="M97" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
       <c r="N97" t="s">
         <v>228</v>
       </c>
       <c r="O97" t="s">
-        <v>412</v>
+        <v>407</v>
       </c>
     </row>
     <row r="98" spans="1:15" x14ac:dyDescent="0.25">
@@ -6701,13 +6701,13 @@
         <v>48</v>
       </c>
       <c r="M98" t="s">
+        <v>406</v>
+      </c>
+      <c r="N98" t="s">
+        <v>424</v>
+      </c>
+      <c r="O98" t="s">
         <v>411</v>
-      </c>
-      <c r="N98" t="s">
-        <v>429</v>
-      </c>
-      <c r="O98" t="s">
-        <v>416</v>
       </c>
     </row>
     <row r="99" spans="1:15" x14ac:dyDescent="0.25">
@@ -6748,13 +6748,13 @@
         <v>48</v>
       </c>
       <c r="M99" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
       <c r="N99" t="s">
         <v>120</v>
       </c>
       <c r="O99" t="s">
-        <v>416</v>
+        <v>411</v>
       </c>
     </row>
     <row r="100" spans="1:15" x14ac:dyDescent="0.25">
@@ -6795,13 +6795,13 @@
         <v>48</v>
       </c>
       <c r="M100" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
       <c r="N100" t="s">
         <v>146</v>
       </c>
       <c r="O100" t="s">
-        <v>416</v>
+        <v>411</v>
       </c>
     </row>
     <row r="101" spans="1:15" x14ac:dyDescent="0.25">
@@ -6842,13 +6842,13 @@
         <v>48</v>
       </c>
       <c r="M101" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
       <c r="N101" t="s">
         <v>186</v>
       </c>
       <c r="O101" t="s">
-        <v>416</v>
+        <v>411</v>
       </c>
     </row>
     <row r="102" spans="1:15" x14ac:dyDescent="0.25">
@@ -6889,13 +6889,13 @@
         <v>48</v>
       </c>
       <c r="M102" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
       <c r="N102" t="s">
         <v>203</v>
       </c>
       <c r="O102" t="s">
-        <v>416</v>
+        <v>411</v>
       </c>
     </row>
     <row r="103" spans="1:15" x14ac:dyDescent="0.25">
@@ -6936,13 +6936,13 @@
         <v>48</v>
       </c>
       <c r="M103" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
       <c r="N103" t="s">
         <v>230</v>
       </c>
       <c r="O103" t="s">
-        <v>416</v>
+        <v>411</v>
       </c>
     </row>
     <row r="104" spans="1:15" x14ac:dyDescent="0.25">
@@ -6983,13 +6983,13 @@
         <v>48</v>
       </c>
       <c r="M104" t="s">
+        <v>406</v>
+      </c>
+      <c r="N104" t="s">
+        <v>425</v>
+      </c>
+      <c r="O104" t="s">
         <v>411</v>
-      </c>
-      <c r="N104" t="s">
-        <v>430</v>
-      </c>
-      <c r="O104" t="s">
-        <v>416</v>
       </c>
     </row>
     <row r="105" spans="1:15" x14ac:dyDescent="0.25">
@@ -7030,13 +7030,13 @@
         <v>48</v>
       </c>
       <c r="M105" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
       <c r="N105" t="s">
         <v>321</v>
       </c>
       <c r="O105" t="s">
-        <v>416</v>
+        <v>411</v>
       </c>
     </row>
     <row r="106" spans="1:15" x14ac:dyDescent="0.25">
@@ -7077,13 +7077,13 @@
         <v>53</v>
       </c>
       <c r="M106" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
       <c r="N106" t="s">
-        <v>431</v>
+        <v>426</v>
       </c>
       <c r="O106" t="s">
-        <v>417</v>
+        <v>412</v>
       </c>
     </row>
     <row r="107" spans="1:15" x14ac:dyDescent="0.25">
@@ -7124,13 +7124,13 @@
         <v>53</v>
       </c>
       <c r="M107" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
       <c r="N107" t="s">
-        <v>432</v>
+        <v>427</v>
       </c>
       <c r="O107" t="s">
-        <v>417</v>
+        <v>412</v>
       </c>
     </row>
     <row r="108" spans="1:15" x14ac:dyDescent="0.25">
@@ -7171,13 +7171,13 @@
         <v>53</v>
       </c>
       <c r="M108" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
       <c r="N108" t="s">
         <v>194</v>
       </c>
       <c r="O108" t="s">
-        <v>417</v>
+        <v>412</v>
       </c>
     </row>
     <row r="109" spans="1:15" x14ac:dyDescent="0.25">
@@ -7218,13 +7218,13 @@
         <v>53</v>
       </c>
       <c r="M109" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
       <c r="N109" t="s">
         <v>205</v>
       </c>
       <c r="O109" t="s">
-        <v>417</v>
+        <v>412</v>
       </c>
     </row>
     <row r="110" spans="1:15" x14ac:dyDescent="0.25">
@@ -7265,13 +7265,13 @@
         <v>53</v>
       </c>
       <c r="M110" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
       <c r="N110" t="s">
         <v>232</v>
       </c>
       <c r="O110" t="s">
-        <v>417</v>
+        <v>412</v>
       </c>
     </row>
     <row r="111" spans="1:15" x14ac:dyDescent="0.25">
@@ -7312,13 +7312,13 @@
         <v>53</v>
       </c>
       <c r="M111" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
       <c r="N111" t="s">
         <v>297</v>
       </c>
       <c r="O111" t="s">
-        <v>417</v>
+        <v>412</v>
       </c>
     </row>
     <row r="112" spans="1:15" x14ac:dyDescent="0.25">
@@ -7359,13 +7359,13 @@
         <v>73</v>
       </c>
       <c r="M112" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
       <c r="N112" t="s">
-        <v>433</v>
+        <v>428</v>
       </c>
       <c r="O112" t="s">
-        <v>418</v>
+        <v>413</v>
       </c>
     </row>
     <row r="113" spans="1:15" x14ac:dyDescent="0.25">
@@ -7406,13 +7406,13 @@
         <v>73</v>
       </c>
       <c r="M113" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
       <c r="N113" t="s">
         <v>132</v>
       </c>
       <c r="O113" t="s">
-        <v>418</v>
+        <v>413</v>
       </c>
     </row>
     <row r="114" spans="1:15" x14ac:dyDescent="0.25">
@@ -7453,13 +7453,13 @@
         <v>73</v>
       </c>
       <c r="M114" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
       <c r="N114" t="s">
         <v>158</v>
       </c>
       <c r="O114" t="s">
-        <v>418</v>
+        <v>413</v>
       </c>
     </row>
     <row r="115" spans="1:15" x14ac:dyDescent="0.25">
@@ -7500,13 +7500,13 @@
         <v>73</v>
       </c>
       <c r="M115" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
       <c r="N115" t="s">
         <v>220</v>
       </c>
       <c r="O115" t="s">
-        <v>418</v>
+        <v>413</v>
       </c>
     </row>
     <row r="116" spans="1:15" x14ac:dyDescent="0.25">
@@ -7547,13 +7547,13 @@
         <v>73</v>
       </c>
       <c r="M116" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
       <c r="N116" t="s">
         <v>255</v>
       </c>
       <c r="O116" t="s">
-        <v>418</v>
+        <v>413</v>
       </c>
     </row>
     <row r="117" spans="1:15" x14ac:dyDescent="0.25">
@@ -7594,13 +7594,13 @@
         <v>73</v>
       </c>
       <c r="M117" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
       <c r="N117" t="s">
         <v>295</v>
       </c>
       <c r="O117" t="s">
-        <v>418</v>
+        <v>413</v>
       </c>
     </row>
     <row r="118" spans="1:15" x14ac:dyDescent="0.25">
@@ -8279,6 +8279,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:O132" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:O132">
     <sortCondition ref="J2:J132"/>
   </sortState>

</xml_diff>